<commit_message>
Changed output format to CSV for PDF inputs
</commit_message>
<xml_diff>
--- a/Output/JABG31P037_Lang_OUTPUT.xlsx
+++ b/Output/JABG31P037_Lang_OUTPUT.xlsx
@@ -1,69 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Verbatim</t>
-  </si>
-  <si>
-    <t>Genus</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Authorship</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Goodenia asteriscus P.J.Lang,</t>
-  </si>
-  <si>
-    <t>Goodenia</t>
-  </si>
-  <si>
-    <t>asteriscus</t>
-  </si>
-  <si>
-    <t>P. J. Lang</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -78,35 +46,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -394,45 +353,473 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>kindOfName</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>scientificName</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>taxonomicNameStringWithAuthor</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>cultivarNameGroup</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>verbatim</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>uninomial</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>genus</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>combinationAuthorship</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>basionymAuthorship</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>namePublishedInYear</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>combinationExAuthorship</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>taxonRank</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>verbatimTaxonRank</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>nomenclaturalCode</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>taxonomicName</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>protonym</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>accordingTo</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>basionym</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>nameAccordingTo</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>infragenericEpithet</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>specificEpithet</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>infraspecificEpithet</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>scientificNameAuthorship</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Goodenia sp. aff. quasilibera (Davies &amp; Alford 2012).</t>
+        </is>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>genus</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>genus</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Goodenia sp. affin. quasilibera (L. Ransom 868 R.J.Davies &amp; J.Alford, Metals X Ltd Wingellina Nickel Proj. Level 1 Fl. &amp;</t>
+        </is>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>genus</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>genus</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Goodenia asteriscus</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Goodenia asteriscus P.J.Lang,</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Goodenia</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>specificEpithet</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>specificEpithet</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>Goodenia asteriscus P. J. Lang</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>asteriscus</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>P. J. Lang</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
         <v>7</v>
       </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>